<commit_message>
First functional iteration of BM3DELBP predictor
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Independent-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79FB1CA-680D-4AB6-9631-85CAFAC4304E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55943008-3BA7-4BCE-BE8B-7CE8C4DE6892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
+    <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -526,7 +526,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -893,7 +892,7 @@
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,45 +914,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="35"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="34"/>
       <c r="T1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="28" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="28" t="s">
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="16" t="s">
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="T2" s="10" t="s">
@@ -961,20 +960,20 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="17">
+      <c r="B3" s="12"/>
+      <c r="C3" s="16">
         <v>0.25</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>0.5</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>0.75</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>1</v>
       </c>
       <c r="G3" s="5">
@@ -1009,45 +1008,45 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <v>0.77184151785714195</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>0.81686383928571404</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="24">
         <v>0.76969866071428505</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="24">
         <v>0.80848214285714204</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="25">
         <v>3.5758928571428497E-2</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="27">
+      <c r="H4" s="20"/>
+      <c r="I4" s="26">
         <v>3.6171874999999999E-2</v>
       </c>
-      <c r="J4" s="27">
+      <c r="J4" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="K4" s="27">
-        <v>0.393459821428571</v>
-      </c>
-      <c r="L4" s="27">
-        <v>0.10925223214285699</v>
-      </c>
-      <c r="M4" s="27">
-        <v>0.67265624999999996</v>
-      </c>
-      <c r="N4" s="27">
-        <v>0.68003348214285697</v>
-      </c>
-      <c r="O4" s="27">
+      <c r="K4" s="26">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="L4" s="26">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="M4" s="26">
+        <v>0.32718750000000002</v>
+      </c>
+      <c r="N4" s="26">
+        <v>0.678448660714285</v>
+      </c>
+      <c r="O4" s="26">
         <v>0.74790178571428501</v>
       </c>
       <c r="T4" s="2" t="s">
@@ -1055,45 +1054,45 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>0.77354910714285696</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>0.82244419642857103</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>0.84409598214285697</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>0.82195312499999995</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <v>4.0468749999999998E-2</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="14">
+      <c r="H5" s="21"/>
+      <c r="I5" s="13">
         <v>0.23513392857142801</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <v>3.5591517857142797E-2</v>
       </c>
-      <c r="K5" s="14">
-        <v>0.52720982142857098</v>
-      </c>
-      <c r="L5" s="14">
-        <v>0.15080357142857101</v>
-      </c>
-      <c r="M5" s="14">
-        <v>0.78331473214285696</v>
-      </c>
-      <c r="N5" s="14">
-        <v>0.52792410714285698</v>
-      </c>
-      <c r="O5" s="14">
+      <c r="K5" s="13">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="L5" s="13">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="M5" s="13">
+        <v>0.435926339285714</v>
+      </c>
+      <c r="N5" s="13">
+        <v>0.52712053571428497</v>
+      </c>
+      <c r="O5" s="13">
         <v>0.81271391369047596</v>
       </c>
       <c r="T5" s="3" t="s">
@@ -1101,108 +1100,116 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>0.52756696428571404</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>0.58102678571428501</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>0.59507812500000001</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>0.65741071428571396</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="14">
+      <c r="H6" s="21"/>
+      <c r="I6" s="13">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="K6" s="14">
-        <v>0.44286830357142798</v>
-      </c>
-      <c r="L6" s="14">
-        <v>0.238270089285714</v>
-      </c>
-      <c r="M6" s="14">
-        <v>0.51889508928571404</v>
-      </c>
-      <c r="N6" s="14">
-        <v>0.187857142857142</v>
-      </c>
-      <c r="O6" s="14">
+      <c r="K6" s="13">
+        <v>6.2053571428571402E-2</v>
+      </c>
+      <c r="L6" s="13">
+        <v>5.5145089285714197E-2</v>
+      </c>
+      <c r="M6" s="13">
+        <v>0.37840401785714201</v>
+      </c>
+      <c r="N6" s="13">
+        <v>0.18966517857142801</v>
+      </c>
+      <c r="O6" s="13">
         <v>0.52964378720238003</v>
       </c>
       <c r="T6" s="3"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>0.90797991071428497</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>0.94188616071428499</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>0.92286830357142802</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>0.92715401785714202</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>5.8035714285714197E-2</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="14">
+      <c r="H7" s="21"/>
+      <c r="I7" s="13">
         <v>0.13468749999999999</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="13">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="14">
+      <c r="K7" s="13">
+        <v>0.91092633928571398</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0.78564732142857097</v>
+      </c>
+      <c r="M7" s="13">
+        <v>0.93553571428571403</v>
+      </c>
+      <c r="N7" s="13">
+        <v>0.93553571428571403</v>
+      </c>
+      <c r="O7" s="13">
         <v>0.85184709821428495</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="31"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K10" s="15"/>
+      <c r="K10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
When multiprocessing, detect the number of physical cores on the system and use that many threads
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55943008-3BA7-4BCE-BE8B-7CE8C4DE6892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B93D467-8321-46F7-980C-5B383748B481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
@@ -147,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +179,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -514,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -526,14 +533,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -575,6 +580,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -892,7 +900,7 @@
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,45 +922,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="34"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="32"/>
       <c r="T1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="27" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="27" t="s">
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="15" t="s">
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="14" t="s">
         <v>16</v>
       </c>
       <c r="T2" s="10" t="s">
@@ -960,20 +968,20 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="16">
+      <c r="B3" s="11"/>
+      <c r="C3" s="15">
         <v>0.25</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <v>0.5</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <v>0.75</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="16">
         <v>1</v>
       </c>
       <c r="G3" s="5">
@@ -1008,45 +1016,45 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="20">
         <v>0.77184151785714195</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="21">
         <v>0.81686383928571404</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="22">
         <v>0.76969866071428505</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="22">
         <v>0.80848214285714204</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="23">
         <v>3.5758928571428497E-2</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="26">
+      <c r="H4" s="18"/>
+      <c r="I4" s="24">
         <v>3.6171874999999999E-2</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="24">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="24">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="24">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="M4" s="26">
+      <c r="M4" s="24">
         <v>0.32718750000000002</v>
       </c>
-      <c r="N4" s="26">
+      <c r="N4" s="24">
         <v>0.678448660714285</v>
       </c>
-      <c r="O4" s="26">
+      <c r="O4" s="24">
         <v>0.74790178571428501</v>
       </c>
       <c r="T4" s="2" t="s">
@@ -1054,45 +1062,45 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="17">
         <v>0.77354910714285696</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.82244419642857103</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>0.84409598214285697</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <v>0.82195312499999995</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>4.0468749999999998E-2</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="13">
+      <c r="H5" s="19"/>
+      <c r="I5" s="12">
         <v>0.23513392857142801</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <v>3.5591517857142797E-2</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="12">
         <v>0.435926339285714</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="12">
         <v>0.52712053571428497</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <v>0.81271391369047596</v>
       </c>
       <c r="T5" s="3" t="s">
@@ -1100,116 +1108,116 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="17">
         <v>0.52756696428571404</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <v>0.58102678571428501</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>0.59507812500000001</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <v>0.65741071428571396</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="13">
+      <c r="H6" s="19"/>
+      <c r="I6" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <v>6.2053571428571402E-2</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="12">
         <v>5.5145089285714197E-2</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="12">
         <v>0.37840401785714201</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="12">
         <v>0.18966517857142801</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="12">
         <v>0.52964378720238003</v>
       </c>
       <c r="T6" s="3"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>0.90797991071428497</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>0.94188616071428499</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>0.92286830357142802</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>0.92715401785714202</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>5.8035714285714197E-2</v>
       </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="13">
+      <c r="H7" s="19"/>
+      <c r="I7" s="12">
         <v>0.13468749999999999</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <v>0.91092633928571398</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="12">
         <v>0.78564732142857097</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="12">
         <v>0.93553571428571403</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="12">
         <v>0.93553571428571403</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="12">
         <v>0.85184709821428495</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="29"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K10" s="14"/>
+      <c r="K10" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Added ability to apply noise to test images too
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B93D467-8321-46F7-980C-5B383748B481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309837B0-BA1C-4295-B2B9-D6F55F197647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Algorithm</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>Normal / Benchmark</t>
+  </si>
+  <si>
+    <t>BM3D gaussian-25 BM3D 30/255</t>
+  </si>
+  <si>
+    <t>Speckle Var=0.04</t>
+  </si>
+  <si>
+    <t>Salt&amp;Pepper 4%</t>
   </si>
 </sst>
 </file>
@@ -191,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +237,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -521,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -547,6 +562,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,9 +598,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8943DC0-93CC-42A9-8475-DFBC80C6B514}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,65 +933,87 @@
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="25" customWidth="1"/>
-    <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" customWidth="1"/>
+    <col min="19" max="20" width="15.5703125" customWidth="1"/>
+    <col min="21" max="22" width="15.28515625" customWidth="1"/>
+    <col min="23" max="23" width="25" customWidth="1"/>
+    <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="30" t="s">
+    <row r="1" spans="1:28" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="32"/>
-      <c r="T1" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="35"/>
+      <c r="AB1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="33" t="s">
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="25" t="s">
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="25" t="s">
+      <c r="N2" s="29"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="14" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="AB2" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11"/>
@@ -984,39 +1029,63 @@
       <c r="F3" s="16">
         <v>1</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="5">
         <v>0.25</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="7">
+      <c r="O3" s="7">
         <v>0.75</v>
       </c>
-      <c r="J3" s="7">
+      <c r="P3" s="7">
         <v>1</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="T3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="U3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="V3" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="W3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
+    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1033,126 +1102,154 @@
         <v>0.80848214285714204</v>
       </c>
       <c r="G4" s="23">
+        <v>0.630479910714285</v>
+      </c>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="23">
         <v>3.5758928571428497E-2</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="24">
+      <c r="N4" s="18"/>
+      <c r="O4" s="24">
         <v>3.6171874999999999E-2</v>
       </c>
-      <c r="J4" s="24">
+      <c r="P4" s="24">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="K4" s="24">
+      <c r="Q4" s="24">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="L4" s="24">
+      <c r="R4" s="24">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="M4" s="24">
-        <v>0.32718750000000002</v>
-      </c>
-      <c r="N4" s="24">
+      <c r="S4" s="24">
+        <v>7.2421874999999997E-2</v>
+      </c>
+      <c r="T4" s="24">
+        <v>3.92299107142857E-2</v>
+      </c>
+      <c r="U4" s="24">
         <v>0.678448660714285</v>
       </c>
-      <c r="O4" s="24">
+      <c r="V4" s="41"/>
+      <c r="W4" s="24">
         <v>0.74790178571428501</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="AB4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
       <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0.52756696428571404</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.58102678571428501</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.59507812500000001</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.65741071428571396</v>
+      </c>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="12">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="N5" s="19"/>
+      <c r="O5" s="12">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="P5" s="12">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>6.2053571428571402E-2</v>
+      </c>
+      <c r="R5" s="12">
+        <v>5.5145089285714197E-2</v>
+      </c>
+      <c r="S5" s="42">
+        <v>0.37840401785714201</v>
+      </c>
+      <c r="T5" s="42"/>
+      <c r="U5" s="12">
+        <v>0.18966517857142801</v>
+      </c>
+      <c r="V5" s="42"/>
+      <c r="W5" s="12">
+        <v>0.52964378720238003</v>
+      </c>
+      <c r="AB5" s="2"/>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32"/>
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C6" s="17">
         <v>0.77354910714285696</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D6" s="12">
         <v>0.82244419642857103</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E6" s="12">
         <v>0.84409598214285697</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F6" s="12">
         <v>0.82195312499999995</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="12">
         <v>4.0468749999999998E-2</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="12">
+      <c r="N6" s="19"/>
+      <c r="O6" s="12">
         <v>0.23513392857142801</v>
       </c>
-      <c r="J5" s="12">
+      <c r="P6" s="12">
         <v>3.5591517857142797E-2</v>
       </c>
-      <c r="K5" s="12">
+      <c r="Q6" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="L5" s="12">
+      <c r="R6" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="M5" s="12">
+      <c r="S6" s="42">
         <v>0.435926339285714</v>
       </c>
-      <c r="N5" s="12">
+      <c r="T6" s="42"/>
+      <c r="U6" s="12">
         <v>0.52712053571428497</v>
       </c>
-      <c r="O5" s="12">
+      <c r="V6" s="42"/>
+      <c r="W6" s="12">
         <v>0.81271391369047596</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="AB6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="17">
-        <v>0.52756696428571404</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0.58102678571428501</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0.59507812500000001</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0.65741071428571396</v>
-      </c>
-      <c r="G6" s="12">
-        <v>3.5714285714285698E-2</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="12">
-        <v>3.5714285714285698E-2</v>
-      </c>
-      <c r="J6" s="12">
-        <v>3.5714285714285698E-2</v>
-      </c>
-      <c r="K6" s="12">
-        <v>6.2053571428571402E-2</v>
-      </c>
-      <c r="L6" s="12">
-        <v>5.5145089285714197E-2</v>
-      </c>
-      <c r="M6" s="12">
-        <v>0.37840401785714201</v>
-      </c>
-      <c r="N6" s="12">
-        <v>0.18966517857142801</v>
-      </c>
-      <c r="O6" s="12">
-        <v>0.52964378720238003</v>
-      </c>
-      <c r="T6" s="3"/>
-    </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
+    <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1168,64 +1265,88 @@
       <c r="F7" s="12">
         <v>0.92715401785714202</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="12">
         <v>5.8035714285714197E-2</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="12">
+      <c r="N7" s="19"/>
+      <c r="O7" s="12">
         <v>0.13468749999999999</v>
       </c>
-      <c r="J7" s="12">
+      <c r="P7" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="K7" s="12">
+      <c r="Q7" s="12">
         <v>0.91092633928571398</v>
       </c>
-      <c r="L7" s="12">
+      <c r="R7" s="12">
         <v>0.78564732142857097</v>
       </c>
-      <c r="M7" s="12">
+      <c r="S7" s="12">
+        <v>0.93053571428571402</v>
+      </c>
+      <c r="T7" s="42"/>
+      <c r="U7" s="12">
         <v>0.93553571428571403</v>
       </c>
-      <c r="N7" s="12">
-        <v>0.93553571428571403</v>
-      </c>
-      <c r="O7" s="12">
+      <c r="V7" s="42"/>
+      <c r="W7" s="12">
         <v>0.85184709821428495</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
+    <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K10" s="13"/>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Q10" s="13"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>0.143136160714285</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:U2"/>
     <mergeCell ref="A3:A9"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C1:W1"/>
+    <mergeCell ref="C2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added no-noise class to noiseclassifier options
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309837B0-BA1C-4295-B2B9-D6F55F197647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E97CB9-38E6-40D7-AF86-E118387861B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
+    <workbookView xWindow="4305" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Algorithm</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Salt&amp;Pepper 4%</t>
+  </si>
+  <si>
+    <t>uni</t>
+  </si>
+  <si>
+    <t>Questionable/Repeat?</t>
   </si>
 </sst>
 </file>
@@ -194,13 +200,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,7 +244,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -562,9 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,10 +610,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8943DC0-93CC-42A9-8475-DFBC80C6B514}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W8" sqref="C8:W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,60 +961,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="35"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="32"/>
       <c r="AB1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="28" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="28" t="s">
+      <c r="N2" s="26"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="39"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="36"/>
       <c r="W2" s="14" t="s">
         <v>16</v>
       </c>
@@ -1013,7 +1023,7 @@
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11"/>
@@ -1044,7 +1054,7 @@
       <c r="K3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="37" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="5">
@@ -1074,7 +1084,7 @@
       <c r="U3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="40" t="s">
+      <c r="V3" s="37" t="s">
         <v>24</v>
       </c>
       <c r="W3" s="4" t="s">
@@ -1085,7 +1095,7 @@
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1104,11 +1114,21 @@
       <c r="G4" s="23">
         <v>0.630479910714285</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
+      <c r="H4" s="23">
+        <v>7.1395089285714197E-2</v>
+      </c>
+      <c r="I4" s="23">
+        <v>0.726897321428571</v>
+      </c>
+      <c r="J4" s="12">
+        <v>9.3850446428571405E-2</v>
+      </c>
+      <c r="K4" s="12">
+        <v>8.7522321428571401E-2</v>
+      </c>
+      <c r="L4" s="12">
+        <v>8.9386160714285706E-2</v>
+      </c>
       <c r="M4" s="23">
         <v>3.5758928571428497E-2</v>
       </c>
@@ -1134,7 +1154,9 @@
       <c r="U4" s="24">
         <v>0.678448660714285</v>
       </c>
-      <c r="V4" s="41"/>
+      <c r="V4" s="24">
+        <v>0.43547991071428499</v>
+      </c>
       <c r="W4" s="24">
         <v>0.74790178571428501</v>
       </c>
@@ -1143,7 +1165,7 @@
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1159,12 +1181,24 @@
       <c r="F5" s="12">
         <v>0.65741071428571396</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
+      <c r="G5" s="12">
+        <v>0.275223214285714</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.115602678571428</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0.23975446428571401</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0.21513392857142799</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0.15738839285714201</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0.13934151785714199</v>
+      </c>
       <c r="M5" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
@@ -1181,21 +1215,25 @@
       <c r="R5" s="12">
         <v>5.5145089285714197E-2</v>
       </c>
-      <c r="S5" s="42">
-        <v>0.37840401785714201</v>
-      </c>
-      <c r="T5" s="42"/>
+      <c r="S5" s="12">
+        <v>0.216104910714285</v>
+      </c>
+      <c r="T5" s="12">
+        <v>0.12060267857142799</v>
+      </c>
       <c r="U5" s="12">
         <v>0.18966517857142801</v>
       </c>
-      <c r="V5" s="42"/>
+      <c r="V5" s="12">
+        <v>0.14992187500000001</v>
+      </c>
       <c r="W5" s="12">
         <v>0.52964378720238003</v>
       </c>
       <c r="AB5" s="2"/>
     </row>
     <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1211,12 +1249,24 @@
       <c r="F6" s="12">
         <v>0.82195312499999995</v>
       </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
+      <c r="G6" s="12">
+        <v>0.75100446428571399</v>
+      </c>
+      <c r="H6" s="12">
+        <v>9.3035714285714194E-2</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0.162276785714285</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0.45821428571428502</v>
+      </c>
+      <c r="K6" s="12">
+        <v>7.6540178571428502E-2</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0.104040178571428</v>
+      </c>
       <c r="M6" s="12">
         <v>4.0468749999999998E-2</v>
       </c>
@@ -1233,14 +1283,18 @@
       <c r="R6" s="12">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="S6" s="42">
-        <v>0.435926339285714</v>
-      </c>
-      <c r="T6" s="42"/>
+      <c r="S6" s="12">
+        <v>7.4241071428571406E-2</v>
+      </c>
+      <c r="T6" s="12">
+        <v>3.5714285714285698E-2</v>
+      </c>
       <c r="U6" s="12">
         <v>0.52712053571428497</v>
       </c>
-      <c r="V6" s="42"/>
+      <c r="V6" s="12">
+        <v>0.289419642857142</v>
+      </c>
       <c r="W6" s="12">
         <v>0.81271391369047596</v>
       </c>
@@ -1249,7 +1303,7 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1265,12 +1319,24 @@
       <c r="F7" s="12">
         <v>0.92715401785714202</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44"/>
+      <c r="G7" s="12">
+        <v>0.93203124999999998</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0.90441964285714205</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0.92535714285714199</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0.92809151785714195</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0.912488839285714</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0.91015625</v>
+      </c>
       <c r="M7" s="12">
         <v>5.8035714285714197E-2</v>
       </c>
@@ -1290,44 +1356,57 @@
       <c r="S7" s="12">
         <v>0.93053571428571402</v>
       </c>
-      <c r="T7" s="42"/>
+      <c r="T7" s="12">
+        <v>0.92069196428571398</v>
+      </c>
       <c r="U7" s="12">
         <v>0.93553571428571403</v>
       </c>
-      <c r="V7" s="42"/>
+      <c r="V7" s="12">
+        <v>0.93832589285714196</v>
+      </c>
       <c r="W7" s="12">
         <v>0.85184709821428495</v>
       </c>
+      <c r="AB7" s="40" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="27"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="39">
+        <v>0.92991071428571404</v>
+      </c>
+      <c r="R8" s="38"/>
+      <c r="S8" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="T8" s="38"/>
+      <c r="U8" s="39">
+        <v>0.84196428571428505</v>
+      </c>
+      <c r="V8" s="38"/>
+      <c r="W8" s="38"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="29"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q10" s="13"/>

</xml_diff>

<commit_message>
Changed NoiseClasifier to classify all types of noise
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E97CB9-38E6-40D7-AF86-E118387861B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B211CA49-E34D-4905-835C-8D36E7ABBEA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
+    <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -932,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8943DC0-93CC-42A9-8475-DFBC80C6B514}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W8" sqref="C8:W8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added missing installation step to README, added diagnostics for RuntimeWarning in MRELBP
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B211CA49-E34D-4905-835C-8D36E7ABBEA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB5B517-F552-467C-A2C2-C7113D676DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Algorithm</t>
   </si>
@@ -152,10 +152,16 @@
     <t>Salt&amp;Pepper 4%</t>
   </si>
   <si>
+    <t>desktop</t>
+  </si>
+  <si>
     <t>uni</t>
   </si>
   <si>
     <t>Questionable/Repeat?</t>
+  </si>
+  <si>
+    <t>error, need to retry</t>
   </si>
 </sst>
 </file>
@@ -244,7 +250,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -573,6 +579,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,16 +622,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8943DC0-93CC-42A9-8475-DFBC80C6B514}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,60 +967,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="32"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="40"/>
       <c r="AB1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="25" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="26"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="25" t="s">
+      <c r="N2" s="34"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="36"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="25"/>
       <c r="W2" s="14" t="s">
         <v>16</v>
       </c>
@@ -1023,7 +1029,7 @@
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="37" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11"/>
@@ -1054,7 +1060,7 @@
       <c r="K3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="26" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="5">
@@ -1084,7 +1090,7 @@
       <c r="U3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="37" t="s">
+      <c r="V3" s="26" t="s">
         <v>24</v>
       </c>
       <c r="W3" s="4" t="s">
@@ -1095,7 +1101,7 @@
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1165,7 +1171,7 @@
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1233,7 +1239,7 @@
       <c r="AB5" s="2"/>
     </row>
     <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1303,7 +1309,7 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1368,45 +1374,79 @@
       <c r="W7" s="12">
         <v>0.85184709821428495</v>
       </c>
-      <c r="AB7" s="40" t="s">
-        <v>26</v>
+      <c r="AB7" s="28" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="39">
+      <c r="C8" s="30">
+        <v>0.74972098214285698</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="27">
+        <v>0.66551339285714195</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="27">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="N8" s="29"/>
+      <c r="O8" s="27">
+        <v>0.28069196428571402</v>
+      </c>
+      <c r="P8" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="27">
         <v>0.92991071428571404</v>
       </c>
-      <c r="R8" s="38"/>
-      <c r="S8" s="43" t="s">
+      <c r="R8" s="27">
+        <v>0.21473214285714201</v>
+      </c>
+      <c r="S8" s="27">
+        <v>0.85323660714285698</v>
+      </c>
+      <c r="T8" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="T8" s="38"/>
-      <c r="U8" s="39">
+      <c r="U8" s="27">
         <v>0.84196428571428505</v>
       </c>
-      <c r="V8" s="38"/>
-      <c r="W8" s="38"/>
+      <c r="V8" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="W8" s="31" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="37"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q10" s="13"/>

</xml_diff>

<commit_message>
Fixed a mistake when converting from DatasetManager.Image to BM3DELBP.BM3DELBPImage during multithreaded describe_noise() where both image types existed in memory, hence consumed double the necessary RAM
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB5B517-F552-467C-A2C2-C7113D676DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ACB22D-F5DD-4940-8BDF-79CC9DA3AA97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Algorithm</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Normal / Benchmark</t>
   </si>
   <si>
-    <t>BM3D gaussian-25 BM3D 30/255</t>
-  </si>
-  <si>
     <t>Speckle Var=0.04</t>
   </si>
   <si>
@@ -161,7 +158,13 @@
     <t>Questionable/Repeat?</t>
   </si>
   <si>
-    <t>error, need to retry</t>
+    <t>uni (needs rerunning)</t>
+  </si>
+  <si>
+    <t>CSV / Confusion Matrix Missing</t>
+  </si>
+  <si>
+    <t>laptop</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +263,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -553,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -566,19 +581,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,9 +594,21 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -936,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8943DC0-93CC-42A9-8475-DFBC80C6B514}">
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,61 +987,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="40"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="45"/>
       <c r="AB1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="33" t="s">
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="33" t="s">
+      <c r="N2" s="39"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="14" t="s">
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="13" t="s">
         <v>16</v>
       </c>
       <c r="AB2" s="10" t="s">
@@ -1029,20 +1049,20 @@
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>0.25</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>0.5</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>0.75</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <v>1</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -1055,13 +1075,13 @@
         <v>5</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="26" t="s">
-        <v>24</v>
+      <c r="L3" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="M3" s="5">
         <v>0.25</v>
@@ -1085,13 +1105,13 @@
         <v>5</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="26" t="s">
-        <v>24</v>
+      <c r="V3" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="W3" s="4" t="s">
         <v>9</v>
@@ -1101,69 +1121,69 @@
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="25">
         <v>0.77184151785714195</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="26">
         <v>0.81686383928571404</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="28">
         <v>0.76969866071428505</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="28">
         <v>0.80848214285714204</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="29">
         <v>0.630479910714285</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="29">
         <v>7.1395089285714197E-2</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="29">
         <v>0.726897321428571</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="30">
         <v>9.3850446428571405E-2</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="30">
         <v>8.7522321428571401E-2</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="30">
         <v>8.9386160714285706E-2</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4" s="29">
         <v>3.5758928571428497E-2</v>
       </c>
-      <c r="N4" s="18"/>
-      <c r="O4" s="24">
+      <c r="N4" s="16"/>
+      <c r="O4" s="31">
         <v>3.6171874999999999E-2</v>
       </c>
-      <c r="P4" s="24">
+      <c r="P4" s="31">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="Q4" s="24">
+      <c r="Q4" s="32">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="R4" s="24">
+      <c r="R4" s="31">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="S4" s="24">
+      <c r="S4" s="31">
         <v>7.2421874999999997E-2</v>
       </c>
-      <c r="T4" s="24">
+      <c r="T4" s="31">
         <v>3.92299107142857E-2</v>
       </c>
-      <c r="U4" s="24">
+      <c r="U4" s="31">
         <v>0.678448660714285</v>
       </c>
-      <c r="V4" s="24">
+      <c r="V4" s="31">
         <v>0.43547991071428499</v>
       </c>
-      <c r="W4" s="24">
+      <c r="W4" s="31">
         <v>0.74790178571428501</v>
       </c>
       <c r="AB4" s="2" t="s">
@@ -1171,137 +1191,137 @@
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="33">
         <v>0.52756696428571404</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="30">
         <v>0.58102678571428501</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="30">
         <v>0.59507812500000001</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="30">
         <v>0.65741071428571396</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="34">
         <v>0.275223214285714</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="34">
         <v>0.115602678571428</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="34">
         <v>0.23975446428571401</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="34">
         <v>0.21513392857142799</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="34">
         <v>0.15738839285714201</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="34">
         <v>0.13934151785714199</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="30">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="N5" s="19"/>
-      <c r="O5" s="12">
+      <c r="N5" s="17"/>
+      <c r="O5" s="30">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="P5" s="12">
+      <c r="P5" s="30">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="Q5" s="12">
+      <c r="Q5" s="30">
         <v>6.2053571428571402E-2</v>
       </c>
-      <c r="R5" s="12">
+      <c r="R5" s="30">
         <v>5.5145089285714197E-2</v>
       </c>
-      <c r="S5" s="12">
+      <c r="S5" s="34">
         <v>0.216104910714285</v>
       </c>
-      <c r="T5" s="12">
+      <c r="T5" s="34">
         <v>0.12060267857142799</v>
       </c>
-      <c r="U5" s="12">
+      <c r="U5" s="30">
         <v>0.18966517857142801</v>
       </c>
-      <c r="V5" s="12">
+      <c r="V5" s="34">
         <v>0.14992187500000001</v>
       </c>
-      <c r="W5" s="12">
+      <c r="W5" s="30">
         <v>0.52964378720238003</v>
       </c>
       <c r="AB5" s="2"/>
     </row>
     <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="33">
         <v>0.77354910714285696</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="30">
         <v>0.82244419642857103</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="30">
         <v>0.84409598214285697</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="30">
         <v>0.82195312499999995</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="30">
         <v>0.75100446428571399</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="30">
         <v>9.3035714285714194E-2</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="30">
         <v>0.162276785714285</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="30">
         <v>0.45821428571428502</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="30">
         <v>7.6540178571428502E-2</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="30">
         <v>0.104040178571428</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="30">
         <v>4.0468749999999998E-2</v>
       </c>
-      <c r="N6" s="19"/>
-      <c r="O6" s="12">
+      <c r="N6" s="17"/>
+      <c r="O6" s="30">
         <v>0.23513392857142801</v>
       </c>
-      <c r="P6" s="12">
+      <c r="P6" s="30">
         <v>3.5591517857142797E-2</v>
       </c>
-      <c r="Q6" s="12">
+      <c r="Q6" s="30">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="R6" s="12">
+      <c r="R6" s="30">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="S6" s="12">
+      <c r="S6" s="34">
         <v>7.4241071428571406E-2</v>
       </c>
-      <c r="T6" s="12">
+      <c r="T6" s="34">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="U6" s="12">
+      <c r="U6" s="30">
         <v>0.52712053571428497</v>
       </c>
-      <c r="V6" s="12">
+      <c r="V6" s="30">
         <v>0.289419642857142</v>
       </c>
-      <c r="W6" s="12">
+      <c r="W6" s="30">
         <v>0.81271391369047596</v>
       </c>
       <c r="AB6" s="3" t="s">
@@ -1309,155 +1329,150 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="34">
         <v>0.90797991071428497</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="30">
         <v>0.94188616071428499</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="34">
         <v>0.92286830357142802</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="34">
         <v>0.92715401785714202</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="30">
         <v>0.93203124999999998</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="30">
         <v>0.90441964285714205</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="30">
         <v>0.92535714285714199</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="30">
         <v>0.92809151785714195</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="30">
         <v>0.912488839285714</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="30">
         <v>0.91015625</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="34">
         <v>5.8035714285714197E-2</v>
       </c>
-      <c r="N7" s="19"/>
-      <c r="O7" s="12">
+      <c r="N7" s="17"/>
+      <c r="O7" s="34">
         <v>0.13468749999999999</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="34">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="Q7" s="30">
         <v>0.91092633928571398</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="34">
         <v>0.78564732142857097</v>
       </c>
-      <c r="S7" s="12">
+      <c r="S7" s="30">
         <v>0.93053571428571402</v>
       </c>
-      <c r="T7" s="12">
+      <c r="T7" s="34">
         <v>0.92069196428571398</v>
       </c>
-      <c r="U7" s="12">
+      <c r="U7" s="34">
         <v>0.93553571428571403</v>
       </c>
-      <c r="V7" s="12">
+      <c r="V7" s="34">
         <v>0.93832589285714196</v>
       </c>
-      <c r="W7" s="12">
+      <c r="W7" s="30">
         <v>0.85184709821428495</v>
       </c>
-      <c r="AB7" s="28" t="s">
-        <v>27</v>
+      <c r="AB7" s="21" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="35">
         <v>0.74972098214285698</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="36">
+        <v>0.78465401785714195</v>
+      </c>
+      <c r="E8" s="36">
+        <v>0.822600446428571</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="20">
+        <v>0.66551339285714195</v>
+      </c>
+      <c r="H8" s="20">
+        <v>0.96333705357142796</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="36">
+        <v>0.72868303571428505</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="36">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="N8" s="22"/>
+      <c r="O8" s="36">
+        <v>0.28069196428571402</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="36">
+        <v>0.92991071428571404</v>
+      </c>
+      <c r="R8" s="37">
+        <v>0.21473214285714201</v>
+      </c>
+      <c r="S8" s="36">
+        <v>0.85323660714285698</v>
+      </c>
+      <c r="T8" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="U8" s="36">
+        <v>0.84196428571428505</v>
+      </c>
+      <c r="V8" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="W8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB8" s="27" t="s">
         <v>28</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="27">
-        <v>0.66551339285714195</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" s="27">
-        <v>3.5714285714285698E-2</v>
-      </c>
-      <c r="N8" s="29"/>
-      <c r="O8" s="27">
-        <v>0.28069196428571402</v>
-      </c>
-      <c r="P8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q8" s="27">
-        <v>0.92991071428571404</v>
-      </c>
-      <c r="R8" s="27">
-        <v>0.21473214285714201</v>
-      </c>
-      <c r="S8" s="27">
-        <v>0.85323660714285698</v>
-      </c>
-      <c r="T8" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="U8" s="27">
-        <v>0.84196428571428505</v>
-      </c>
-      <c r="V8" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="W8" s="31" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
+      <c r="A9" s="42"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q10" s="13"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13">
-        <v>0.143136160714285</v>
-      </c>
+      <c r="Q10" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Diagnostics for strange rotation issue
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ACA267-AF44-418B-9B27-DF3046DDC279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A7EDB9-2834-4952-830D-53FB433E790D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
+    <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Algorithm</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Rotation Invariance (50%)</t>
   </si>
   <si>
-    <t>Normal (50%)</t>
-  </si>
-  <si>
     <t>Model Trained &amp; Results</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
   </si>
   <si>
     <t>CSV / Confusion Matrix Missing</t>
-  </si>
-  <si>
-    <t>laptop</t>
   </si>
 </sst>
 </file>
@@ -214,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,12 +241,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -568,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -585,28 +573,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -640,7 +625,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -955,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8943DC0-93CC-42A9-8475-DFBC80C6B514}">
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,80 +959,78 @@
     <col min="11" max="11" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" customWidth="1"/>
-    <col min="14" max="15" width="13" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" customWidth="1"/>
-    <col min="19" max="20" width="15.5703125" customWidth="1"/>
-    <col min="21" max="22" width="15.28515625" customWidth="1"/>
-    <col min="23" max="23" width="25" customWidth="1"/>
-    <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
+    <col min="18" max="19" width="15.5703125" customWidth="1"/>
+    <col min="20" max="21" width="15.28515625" customWidth="1"/>
+    <col min="22" max="22" width="25" customWidth="1"/>
+    <col min="27" max="27" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="41" t="s">
+    <row r="1" spans="1:27" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="43"/>
-      <c r="AB1" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="40"/>
+      <c r="AA1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="36" t="s">
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="37"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="36" t="s">
+      <c r="N2" s="35"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="13" t="s">
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AB2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11"/>
@@ -1074,411 +1056,403 @@
         <v>5</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="19" t="s">
-        <v>23</v>
+      <c r="L3" s="17" t="s">
+        <v>22</v>
       </c>
       <c r="M3" s="5">
         <v>0.25</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>17</v>
+      <c r="N3" s="7">
+        <v>0.75</v>
       </c>
       <c r="O3" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="P3" s="7">
         <v>1</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>4</v>
       </c>
+      <c r="Q3" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="R3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="S3" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="S3" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="T3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="U3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="V3" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="W3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="37"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="22">
         <v>0.77184151785714195</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="32">
         <v>0.82091517857142804</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="24">
         <v>0.76969866071428505</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="24">
         <v>0.80848214285714204</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="25">
         <v>0.630479910714285</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="25">
         <v>7.1395089285714197E-2</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="25">
         <v>0.726897321428571</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="26">
         <v>9.3850446428571405E-2</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4" s="26">
         <v>8.7522321428571401E-2</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="26">
         <v>8.9386160714285706E-2</v>
       </c>
-      <c r="M4" s="28">
+      <c r="M4" s="25">
         <v>3.5758928571428497E-2</v>
       </c>
-      <c r="N4" s="16"/>
-      <c r="O4" s="30">
+      <c r="N4" s="27">
         <v>3.6171874999999999E-2</v>
       </c>
-      <c r="P4" s="30">
+      <c r="O4" s="27">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="Q4" s="30">
+      <c r="P4" s="27">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="R4" s="30">
+      <c r="Q4" s="27">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="S4" s="30">
+      <c r="R4" s="27">
         <v>7.2421874999999997E-2</v>
       </c>
-      <c r="T4" s="30">
+      <c r="S4" s="27">
         <v>3.92299107142857E-2</v>
       </c>
-      <c r="U4" s="30">
+      <c r="T4" s="27">
         <v>0.678448660714285</v>
       </c>
-      <c r="V4" s="30">
+      <c r="U4" s="27">
         <v>0.43547991071428499</v>
       </c>
-      <c r="W4" s="30">
+      <c r="V4" s="27">
         <v>0.74790178571428501</v>
       </c>
-      <c r="AB4" s="2" t="s">
+      <c r="AA4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="37"/>
       <c r="B5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="31">
+        <v>19</v>
+      </c>
+      <c r="C5" s="28">
         <v>0.52756696428571404</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="26">
         <v>0.58102678571428501</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="26">
         <v>0.59507812500000001</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="26">
         <v>0.65741071428571396</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="26">
         <v>0.275223214285714</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="26">
         <v>8.1551339285714203E-2</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="26">
         <v>0.147555803571428</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="26">
         <v>0.123950892857142</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="26">
         <v>9.4944196428571395E-2</v>
       </c>
-      <c r="L5" s="29">
+      <c r="L5" s="26">
         <v>7.9765625000000007E-2</v>
       </c>
-      <c r="M5" s="29">
+      <c r="M5" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="29">
+      <c r="N5" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="P5" s="29">
+      <c r="O5" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="Q5" s="29">
+      <c r="P5" s="26">
         <v>6.2053571428571402E-2</v>
       </c>
-      <c r="R5" s="29">
+      <c r="Q5" s="26">
         <v>5.5145089285714197E-2</v>
       </c>
-      <c r="S5" s="32">
-        <v>0.216104910714285</v>
-      </c>
-      <c r="T5" s="32">
-        <v>0.12060267857142799</v>
-      </c>
-      <c r="U5" s="29">
+      <c r="R5" s="26">
+        <v>0.143649553571428</v>
+      </c>
+      <c r="S5" s="26">
+        <v>0.10940848214285701</v>
+      </c>
+      <c r="T5" s="26">
         <v>0.18966517857142801</v>
       </c>
-      <c r="V5" s="29">
+      <c r="U5" s="26">
         <v>7.5792410714285705E-2</v>
       </c>
-      <c r="W5" s="29">
+      <c r="V5" s="26">
         <v>0.52964378720238003</v>
       </c>
-      <c r="AB5" s="2"/>
+      <c r="AA5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
+    <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="37"/>
       <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="31">
+        <v>18</v>
+      </c>
+      <c r="C6" s="28">
         <v>0.77354910714285696</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="26">
         <v>0.82244419642857103</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="26">
         <v>0.84409598214285697</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="26">
         <v>0.82195312499999995</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="26">
         <v>0.75100446428571399</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="26">
         <v>9.3035714285714194E-2</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="26">
         <v>0.162276785714285</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="26">
         <v>0.45821428571428502</v>
       </c>
-      <c r="K6" s="29">
+      <c r="K6" s="26">
         <v>7.6540178571428502E-2</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="26">
         <v>0.104040178571428</v>
       </c>
-      <c r="M6" s="29">
+      <c r="M6" s="26">
         <v>4.0468749999999998E-2</v>
       </c>
-      <c r="N6" s="17"/>
-      <c r="O6" s="29">
+      <c r="N6" s="26">
         <v>0.23513392857142801</v>
       </c>
-      <c r="P6" s="29">
+      <c r="O6" s="26">
         <v>3.5591517857142797E-2</v>
       </c>
-      <c r="Q6" s="29">
+      <c r="P6" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="R6" s="29">
+      <c r="Q6" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="S6" s="32">
-        <v>7.4241071428571406E-2</v>
-      </c>
-      <c r="T6" s="32">
+      <c r="R6" s="26">
+        <v>6.6718749999999993E-2</v>
+      </c>
+      <c r="S6" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="U6" s="29">
+      <c r="T6" s="26">
         <v>0.52712053571428497</v>
       </c>
-      <c r="V6" s="29">
+      <c r="U6" s="26">
         <v>0.289419642857142</v>
       </c>
-      <c r="W6" s="29">
+      <c r="V6" s="26">
         <v>0.81271391369047596</v>
       </c>
-      <c r="AB6" s="3" t="s">
-        <v>18</v>
+      <c r="AA6" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
+    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="26">
         <v>0.91660714285714195</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="26">
         <v>0.94188616071428499</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="26">
         <v>0.92286830357142802</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="26">
         <v>0.92715401785714202</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="26">
         <v>0.93203124999999998</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="26">
         <v>0.90441964285714205</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="26">
         <v>0.92535714285714199</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="26">
         <v>0.92809151785714195</v>
       </c>
-      <c r="K7" s="29">
+      <c r="K7" s="26">
         <v>0.912488839285714</v>
       </c>
-      <c r="L7" s="29">
+      <c r="L7" s="26">
         <v>0.91015625</v>
       </c>
-      <c r="M7" s="29">
+      <c r="M7" s="26">
         <v>5.68080357142857E-2</v>
       </c>
-      <c r="N7" s="17"/>
-      <c r="O7" s="29">
+      <c r="N7" s="26">
         <v>0.14849330357142801</v>
       </c>
-      <c r="P7" s="29">
+      <c r="O7" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="Q7" s="29">
+      <c r="P7" s="26">
         <v>0.91092633928571398</v>
       </c>
-      <c r="R7" s="29">
+      <c r="Q7" s="26">
         <v>0.785680803571428</v>
       </c>
-      <c r="S7" s="29">
+      <c r="R7" s="26">
         <v>0.93053571428571402</v>
       </c>
-      <c r="T7" s="29">
+      <c r="S7" s="26">
         <v>0.92069196428571398</v>
       </c>
-      <c r="U7" s="29">
+      <c r="T7" s="26">
         <v>0.93553571428571403</v>
       </c>
-      <c r="V7" s="29">
+      <c r="U7" s="26">
         <v>0.93831473214285699</v>
       </c>
-      <c r="W7" s="29">
+      <c r="V7" s="26">
         <v>0.85184709821428495</v>
       </c>
-      <c r="AB7" s="21" t="s">
-        <v>26</v>
+      <c r="AA7" s="19" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
+    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="37"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="29">
         <v>0.74972098214285698</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="30">
         <v>0.78465401785714195</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="30">
         <v>0.822600446428571</v>
       </c>
-      <c r="F8" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="20">
+      <c r="F8" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="18">
         <v>0.66551339285714195</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="18">
         <v>0.96333705357142796</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="30">
+        <v>0.72868303571428505</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="30">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="N8" s="30">
+        <v>0.28069196428571402</v>
+      </c>
+      <c r="O8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="30">
+        <v>0.92991071428571404</v>
+      </c>
+      <c r="Q8" s="31">
+        <v>0.21473214285714201</v>
+      </c>
+      <c r="R8" s="30">
+        <v>0.85323660714285698</v>
+      </c>
+      <c r="S8" s="31">
+        <v>0.124274553571428</v>
+      </c>
+      <c r="T8" s="30">
+        <v>0.84196428571428505</v>
+      </c>
+      <c r="U8" s="31">
+        <v>0.84787946428571404</v>
+      </c>
+      <c r="V8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA8" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="34">
-        <v>0.72868303571428505</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="34">
-        <v>3.5714285714285698E-2</v>
-      </c>
-      <c r="N8" s="22"/>
-      <c r="O8" s="34">
-        <v>0.28069196428571402</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q8" s="34">
-        <v>0.92991071428571404</v>
-      </c>
-      <c r="R8" s="35">
-        <v>0.21473214285714201</v>
-      </c>
-      <c r="S8" s="34">
-        <v>0.85323660714285698</v>
-      </c>
-      <c r="T8" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="U8" s="34">
-        <v>0.84196428571428505</v>
-      </c>
-      <c r="V8" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="W8" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB8" s="26" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q10" s="12"/>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P10" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:T2"/>
     <mergeCell ref="A3:A9"/>
-    <mergeCell ref="C1:W1"/>
+    <mergeCell ref="C1:V1"/>
     <mergeCell ref="C2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Only use maxtasksperchild if classifying rotations of textures. Improve making of directories in SARBM3D
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A7EDB9-2834-4952-830D-53FB433E790D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F839339-42C8-4B83-A3A6-967BBB3DE15C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
+    <workbookView xWindow="29580" yWindow="-6405" windowWidth="21600" windowHeight="11385" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -577,7 +577,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -595,13 +594,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -941,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8943DC0-93CC-42A9-8475-DFBC80C6B514}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,57 +969,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="40"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="39"/>
       <c r="AA1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="33" t="s">
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="33" t="s">
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="36"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="34"/>
       <c r="U2" s="16"/>
       <c r="V2" s="13" t="s">
         <v>16</v>
@@ -1030,7 +1029,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11"/>
@@ -1099,68 +1098,68 @@
       </c>
     </row>
     <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <v>0.77184151785714195</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <v>0.82091517857142804</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>0.76969866071428505</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>0.80848214285714204</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="24">
         <v>0.630479910714285</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="24">
         <v>7.1395089285714197E-2</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="24">
         <v>0.726897321428571</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="25">
         <v>9.3850446428571405E-2</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="25">
         <v>8.7522321428571401E-2</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="25">
         <v>8.9386160714285706E-2</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4" s="24">
         <v>3.5758928571428497E-2</v>
       </c>
-      <c r="N4" s="27">
+      <c r="N4" s="26">
         <v>3.6171874999999999E-2</v>
       </c>
-      <c r="O4" s="27">
+      <c r="O4" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="P4" s="27">
+      <c r="P4" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="Q4" s="27">
+      <c r="Q4" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="R4" s="27">
+      <c r="R4" s="26">
         <v>7.2421874999999997E-2</v>
       </c>
-      <c r="S4" s="27">
+      <c r="S4" s="26">
         <v>3.92299107142857E-2</v>
       </c>
-      <c r="T4" s="27">
+      <c r="T4" s="26">
         <v>0.678448660714285</v>
       </c>
-      <c r="U4" s="27">
+      <c r="U4" s="26">
         <v>0.43547991071428499</v>
       </c>
-      <c r="V4" s="27">
+      <c r="V4" s="26">
         <v>0.74790178571428501</v>
       </c>
       <c r="AA4" s="2" t="s">
@@ -1168,135 +1167,135 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="27">
         <v>0.52756696428571404</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>0.58102678571428501</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>0.59507812500000001</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>0.65741071428571396</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>0.275223214285714</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="25">
         <v>8.1551339285714203E-2</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="25">
         <v>0.147555803571428</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="25">
         <v>0.123950892857142</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="25">
         <v>9.4944196428571395E-2</v>
       </c>
-      <c r="L5" s="26">
+      <c r="L5" s="25">
         <v>7.9765625000000007E-2</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="25">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="N5" s="26">
+      <c r="N5" s="25">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="O5" s="26">
+      <c r="O5" s="25">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="P5" s="26">
+      <c r="P5" s="25">
         <v>6.2053571428571402E-2</v>
       </c>
-      <c r="Q5" s="26">
+      <c r="Q5" s="25">
         <v>5.5145089285714197E-2</v>
       </c>
-      <c r="R5" s="26">
+      <c r="R5" s="25">
         <v>0.143649553571428</v>
       </c>
-      <c r="S5" s="26">
+      <c r="S5" s="25">
         <v>0.10940848214285701</v>
       </c>
-      <c r="T5" s="26">
+      <c r="T5" s="25">
         <v>0.18966517857142801</v>
       </c>
-      <c r="U5" s="26">
+      <c r="U5" s="25">
         <v>7.5792410714285705E-2</v>
       </c>
-      <c r="V5" s="26">
+      <c r="V5" s="25">
         <v>0.52964378720238003</v>
       </c>
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="27">
         <v>0.77354910714285696</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="25">
         <v>0.82244419642857103</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="25">
         <v>0.84409598214285697</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="25">
         <v>0.82195312499999995</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="25">
         <v>0.75100446428571399</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="25">
         <v>9.3035714285714194E-2</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="25">
         <v>0.162276785714285</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="25">
         <v>0.45821428571428502</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="25">
         <v>7.6540178571428502E-2</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="25">
         <v>0.104040178571428</v>
       </c>
-      <c r="M6" s="26">
+      <c r="M6" s="25">
         <v>4.0468749999999998E-2</v>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="25">
         <v>0.23513392857142801</v>
       </c>
-      <c r="O6" s="26">
+      <c r="O6" s="25">
         <v>3.5591517857142797E-2</v>
       </c>
-      <c r="P6" s="26">
+      <c r="P6" s="25">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="Q6" s="26">
+      <c r="Q6" s="25">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="R6" s="26">
+      <c r="R6" s="25">
         <v>6.6718749999999993E-2</v>
       </c>
-      <c r="S6" s="26">
+      <c r="S6" s="25">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="T6" s="26">
+      <c r="T6" s="25">
         <v>0.52712053571428497</v>
       </c>
-      <c r="U6" s="26">
+      <c r="U6" s="25">
         <v>0.289419642857142</v>
       </c>
-      <c r="V6" s="26">
+      <c r="V6" s="25">
         <v>0.81271391369047596</v>
       </c>
       <c r="AA6" s="3" t="s">
@@ -1304,145 +1303,145 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <v>0.91660714285714195</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="25">
         <v>0.94188616071428499</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="25">
         <v>0.92286830357142802</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="25">
         <v>0.92715401785714202</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="25">
         <v>0.93203124999999998</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="25">
         <v>0.90441964285714205</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <v>0.92535714285714199</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="25">
         <v>0.92809151785714195</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="25">
         <v>0.912488839285714</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L7" s="25">
         <v>0.91015625</v>
       </c>
-      <c r="M7" s="26">
+      <c r="M7" s="25">
         <v>5.68080357142857E-2</v>
       </c>
-      <c r="N7" s="26">
+      <c r="N7" s="25">
         <v>0.14849330357142801</v>
       </c>
-      <c r="O7" s="26">
+      <c r="O7" s="25">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="25">
         <v>0.91092633928571398</v>
       </c>
-      <c r="Q7" s="26">
+      <c r="Q7" s="25">
         <v>0.785680803571428</v>
       </c>
-      <c r="R7" s="26">
+      <c r="R7" s="25">
         <v>0.93053571428571402</v>
       </c>
-      <c r="S7" s="26">
+      <c r="S7" s="25">
         <v>0.92069196428571398</v>
       </c>
-      <c r="T7" s="26">
+      <c r="T7" s="25">
         <v>0.93553571428571403</v>
       </c>
-      <c r="U7" s="26">
+      <c r="U7" s="25">
         <v>0.93831473214285699</v>
       </c>
-      <c r="V7" s="26">
+      <c r="V7" s="25">
         <v>0.85184709821428495</v>
       </c>
-      <c r="AA7" s="19" t="s">
+      <c r="AA7" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="28">
         <v>0.74972098214285698</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <v>0.78465401785714195</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <v>0.822600446428571</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="29">
         <v>0.66551339285714195</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="30">
         <v>0.96333705357142796</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="29">
         <v>0.72868303571428505</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="30">
+      <c r="M8" s="29">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="N8" s="30">
+      <c r="N8" s="29">
         <v>0.28069196428571402</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="30">
+      <c r="P8" s="29">
         <v>0.92991071428571404</v>
       </c>
-      <c r="Q8" s="31">
-        <v>0.21473214285714201</v>
-      </c>
-      <c r="R8" s="30">
+      <c r="Q8" s="29">
+        <v>0.21601562499999999</v>
+      </c>
+      <c r="R8" s="29">
         <v>0.85323660714285698</v>
       </c>
-      <c r="S8" s="31">
-        <v>0.124274553571428</v>
-      </c>
-      <c r="T8" s="30">
+      <c r="S8" s="29">
+        <v>0.12756696428571401</v>
+      </c>
+      <c r="T8" s="29">
         <v>0.84196428571428505</v>
       </c>
-      <c r="U8" s="31">
+      <c r="U8" s="30">
         <v>0.84787946428571404</v>
       </c>
-      <c r="V8" s="20" t="s">
+      <c r="V8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AA8" s="23" t="s">
+      <c r="AA8" s="22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
+      <c r="A9" s="36"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="P10" s="12"/>

</xml_diff>

<commit_message>
Fixed error where SARBM3D is not loaded from C drive when on ECS computers
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F839339-42C8-4B83-A3A6-967BBB3DE15C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111E6D78-C124-4307-8CCF-1EBAF1E1C670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="-6405" windowWidth="21600" windowHeight="11385" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
+    <workbookView xWindow="3660" yWindow="2535" windowWidth="21600" windowHeight="11385" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Algorithm</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>Salt&amp;Pepper 4%</t>
-  </si>
-  <si>
-    <t>desktop</t>
   </si>
   <si>
     <t>uni</t>
@@ -940,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8943DC0-93CC-42A9-8475-DFBC80C6B514}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1365,7 @@
         <v>0.85184709821428495</v>
       </c>
       <c r="AA7" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1386,25 +1383,25 @@
         <v>0.822600446428571</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" s="29">
         <v>0.66551339285714195</v>
       </c>
-      <c r="H8" s="30">
-        <v>0.96333705357142796</v>
+      <c r="H8" s="29">
+        <v>0.93906250000000002</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="J8" s="30">
+        <v>0.1140625</v>
       </c>
       <c r="K8" s="29">
         <v>0.72868303571428505</v>
       </c>
-      <c r="L8" s="19" t="s">
-        <v>23</v>
+      <c r="L8" s="29">
+        <v>0.72834821428571395</v>
       </c>
       <c r="M8" s="29">
         <v>3.5714285714285698E-2</v>
@@ -1413,7 +1410,7 @@
         <v>0.28069196428571402</v>
       </c>
       <c r="O8" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P8" s="29">
         <v>0.92991071428571404</v>
@@ -1430,14 +1427,14 @@
       <c r="T8" s="29">
         <v>0.84196428571428505</v>
       </c>
-      <c r="U8" s="30">
+      <c r="U8" s="29">
         <v>0.84787946428571404</v>
       </c>
       <c r="V8" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AA8" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed error affecting SAR-BM3D filter. Fixed some issues with example image generation
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111E6D78-C124-4307-8CCF-1EBAF1E1C670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EC5657-9303-4695-A914-6268FDD9D6D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2535" windowWidth="21600" windowHeight="11385" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
+    <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>Algorithm</t>
   </si>
@@ -146,9 +146,6 @@
     <t>Salt&amp;Pepper 4%</t>
   </si>
   <si>
-    <t>uni</t>
-  </si>
-  <si>
     <t>Questionable/Repeat?</t>
   </si>
   <si>
@@ -156,6 +153,30 @@
   </si>
   <si>
     <t>CSV / Confusion Matrix Missing</t>
+  </si>
+  <si>
+    <t>desktop</t>
+  </si>
+  <si>
+    <t>No Noise</t>
+  </si>
+  <si>
+    <t>Gaussian</t>
+  </si>
+  <si>
+    <t>Speckle</t>
+  </si>
+  <si>
+    <t>Salt &amp; Pepper</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Noise Classifier w/ RBF</t>
+  </si>
+  <si>
+    <t>Noise Classifier w/ Poly</t>
   </si>
 </sst>
 </file>
@@ -205,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +281,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -549,11 +576,90 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -588,7 +694,12 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -621,6 +732,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8943DC0-93CC-42A9-8475-DFBC80C6B514}">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AC26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,79 +1096,83 @@
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" customWidth="1"/>
-    <col min="18" max="19" width="15.5703125" customWidth="1"/>
-    <col min="20" max="21" width="15.28515625" customWidth="1"/>
-    <col min="22" max="22" width="25" customWidth="1"/>
-    <col min="27" max="27" width="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="20" max="21" width="15.5703125" customWidth="1"/>
+    <col min="22" max="23" width="15.28515625" customWidth="1"/>
+    <col min="24" max="24" width="25" customWidth="1"/>
+    <col min="29" max="29" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="37" t="s">
+    <row r="1" spans="1:29" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="39"/>
-      <c r="AA1" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="42"/>
+      <c r="AC1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="40" t="s">
+    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="32" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="32" t="s">
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="13" t="s">
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AA2" s="10" t="s">
+      <c r="AC2" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11"/>
@@ -1063,39 +1209,45 @@
       <c r="M3" s="5">
         <v>0.25</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="O3" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="P3" s="7">
         <v>0.75</v>
       </c>
-      <c r="O3" s="7">
+      <c r="Q3" s="7">
         <v>1</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="U3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="V3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="W3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
+    <row r="4" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1132,39 +1284,45 @@
       <c r="M4" s="24">
         <v>3.5758928571428497E-2</v>
       </c>
-      <c r="N4" s="26">
+      <c r="N4" s="24">
+        <v>0.120658482142857</v>
+      </c>
+      <c r="O4" s="24">
+        <v>0.25041294642857098</v>
+      </c>
+      <c r="P4" s="26">
         <v>3.6171874999999999E-2</v>
-      </c>
-      <c r="O4" s="26">
-        <v>3.5714285714285698E-2</v>
-      </c>
-      <c r="P4" s="26">
-        <v>3.5714285714285698E-2</v>
       </c>
       <c r="Q4" s="26">
         <v>3.5714285714285698E-2</v>
       </c>
       <c r="R4" s="26">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="S4" s="26">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="T4" s="26">
         <v>7.2421874999999997E-2</v>
       </c>
-      <c r="S4" s="26">
+      <c r="U4" s="26">
         <v>3.92299107142857E-2</v>
       </c>
-      <c r="T4" s="26">
+      <c r="V4" s="26">
         <v>0.678448660714285</v>
       </c>
-      <c r="U4" s="26">
+      <c r="W4" s="26">
         <v>0.43547991071428499</v>
       </c>
-      <c r="V4" s="26">
+      <c r="X4" s="26">
         <v>0.74790178571428501</v>
       </c>
-      <c r="AA4" s="2" t="s">
+      <c r="AC4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
+    <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1208,30 +1366,36 @@
         <v>3.5714285714285698E-2</v>
       </c>
       <c r="P5" s="25">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="Q5" s="25">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="R5" s="25">
         <v>6.2053571428571402E-2</v>
       </c>
-      <c r="Q5" s="25">
+      <c r="S5" s="25">
         <v>5.5145089285714197E-2</v>
       </c>
-      <c r="R5" s="25">
+      <c r="T5" s="25">
         <v>0.143649553571428</v>
       </c>
-      <c r="S5" s="25">
+      <c r="U5" s="25">
         <v>0.10940848214285701</v>
       </c>
-      <c r="T5" s="25">
+      <c r="V5" s="25">
         <v>0.18966517857142801</v>
       </c>
-      <c r="U5" s="25">
+      <c r="W5" s="25">
         <v>7.5792410714285705E-2</v>
       </c>
-      <c r="V5" s="25">
+      <c r="X5" s="25">
         <v>0.52964378720238003</v>
       </c>
-      <c r="AA5" s="2"/>
-    </row>
-    <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
+      <c r="AC5" s="2"/>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="39"/>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1269,38 +1433,44 @@
         <v>4.0468749999999998E-2</v>
       </c>
       <c r="N6" s="25">
+        <v>0.16383928571428499</v>
+      </c>
+      <c r="O6" s="25">
+        <v>0.33974330357142801</v>
+      </c>
+      <c r="P6" s="25">
         <v>0.23513392857142801</v>
       </c>
-      <c r="O6" s="25">
+      <c r="Q6" s="25">
         <v>3.5591517857142797E-2</v>
       </c>
-      <c r="P6" s="25">
+      <c r="R6" s="25">
         <v>3.5714285714285698E-2</v>
-      </c>
-      <c r="Q6" s="25">
-        <v>3.5714285714285698E-2</v>
-      </c>
-      <c r="R6" s="25">
-        <v>6.6718749999999993E-2</v>
       </c>
       <c r="S6" s="25">
         <v>3.5714285714285698E-2</v>
       </c>
       <c r="T6" s="25">
+        <v>6.6718749999999993E-2</v>
+      </c>
+      <c r="U6" s="25">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="V6" s="25">
         <v>0.52712053571428497</v>
       </c>
-      <c r="U6" s="25">
+      <c r="W6" s="25">
         <v>0.289419642857142</v>
       </c>
-      <c r="V6" s="25">
+      <c r="X6" s="25">
         <v>0.81271391369047596</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AC6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
+    <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="39"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1338,38 +1508,44 @@
         <v>5.68080357142857E-2</v>
       </c>
       <c r="N7" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="O7" s="25">
+        <v>0.63656250000000003</v>
+      </c>
+      <c r="P7" s="25">
         <v>0.14849330357142801</v>
       </c>
-      <c r="O7" s="25">
+      <c r="Q7" s="25">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="P7" s="25">
+      <c r="R7" s="25">
         <v>0.91092633928571398</v>
       </c>
-      <c r="Q7" s="25">
+      <c r="S7" s="25">
         <v>0.785680803571428</v>
       </c>
-      <c r="R7" s="25">
+      <c r="T7" s="25">
         <v>0.93053571428571402</v>
       </c>
-      <c r="S7" s="25">
+      <c r="U7" s="25">
         <v>0.92069196428571398</v>
       </c>
-      <c r="T7" s="25">
+      <c r="V7" s="25">
         <v>0.93553571428571403</v>
       </c>
-      <c r="U7" s="25">
+      <c r="W7" s="25">
         <v>0.93831473214285699</v>
       </c>
-      <c r="V7" s="25">
+      <c r="X7" s="25">
         <v>0.85184709821428495</v>
       </c>
-      <c r="AA7" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
+      <c r="AC7" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="39"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1382,8 +1558,8 @@
       <c r="E8" s="29">
         <v>0.822600446428571</v>
       </c>
-      <c r="F8" s="20" t="s">
-        <v>23</v>
+      <c r="F8" s="19" t="s">
+        <v>26</v>
       </c>
       <c r="G8" s="29">
         <v>0.66551339285714195</v>
@@ -1392,7 +1568,7 @@
         <v>0.93906250000000002</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J8" s="30">
         <v>0.1140625</v>
@@ -1406,49 +1582,257 @@
       <c r="M8" s="29">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="N8" s="29">
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="29">
         <v>0.28069196428571402</v>
       </c>
-      <c r="O8" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="P8" s="29">
+      <c r="Q8" s="29">
+        <v>0.11289062499999999</v>
+      </c>
+      <c r="R8" s="29">
         <v>0.92991071428571404</v>
       </c>
-      <c r="Q8" s="29">
+      <c r="S8" s="29">
         <v>0.21601562499999999</v>
       </c>
-      <c r="R8" s="29">
+      <c r="T8" s="29">
         <v>0.85323660714285698</v>
       </c>
-      <c r="S8" s="29">
+      <c r="U8" s="29">
         <v>0.12756696428571401</v>
       </c>
-      <c r="T8" s="29">
+      <c r="V8" s="29">
         <v>0.84196428571428505</v>
       </c>
-      <c r="U8" s="29">
+      <c r="W8" s="29">
         <v>0.84787946428571404</v>
       </c>
-      <c r="V8" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA8" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P10" s="12"/>
+      <c r="X8" s="29">
+        <v>0.79827867445054901</v>
+      </c>
+      <c r="AC8" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="R10" s="12"/>
+    </row>
+    <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+    </row>
+    <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="50"/>
+      <c r="I14" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="52">
+        <v>98.43</v>
+      </c>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47">
+        <v>93.11</v>
+      </c>
+      <c r="F15" s="47"/>
+      <c r="G15" s="58">
+        <v>99.18</v>
+      </c>
+      <c r="H15" s="58"/>
+      <c r="I15" s="56">
+        <v>96.909970238095198</v>
+      </c>
+      <c r="J15" s="57"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="I16" s="55"/>
+    </row>
+    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="59"/>
+      <c r="E18" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="45"/>
+      <c r="G18" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="45"/>
+      <c r="I18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="52">
+        <v>98.84</v>
+      </c>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47">
+        <v>86.41</v>
+      </c>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47">
+        <v>97.69</v>
+      </c>
+      <c r="H19" s="47"/>
+      <c r="I19" s="54">
+        <v>94.83</v>
+      </c>
+      <c r="J19" s="56">
+        <v>94.440569196428498</v>
+      </c>
+      <c r="K19" s="57"/>
+    </row>
+    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="55"/>
+    </row>
+    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="50"/>
+      <c r="I21" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="52">
+        <v>100</v>
+      </c>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="F22" s="47"/>
+      <c r="G22" s="58">
+        <v>94.03</v>
+      </c>
+      <c r="H22" s="58"/>
+      <c r="I22" s="56">
+        <v>67.66</v>
+      </c>
+      <c r="J22" s="57"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I23" s="55"/>
+    </row>
+    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="53"/>
+      <c r="G25" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="50"/>
+      <c r="I25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" s="60" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="52">
+        <v>100</v>
+      </c>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47">
+        <v>17.86</v>
+      </c>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47">
+        <v>87.49</v>
+      </c>
+      <c r="H26" s="47"/>
+      <c r="I26" s="54">
+        <v>62.65</v>
+      </c>
+      <c r="J26" s="46">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:T2"/>
+  <mergeCells count="29">
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="R2:V2"/>
     <mergeCell ref="A3:A9"/>
-    <mergeCell ref="C1:V1"/>
+    <mergeCell ref="C1:X1"/>
     <mergeCell ref="C2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added CSVs for test results and PNGs for classification confusion matrixes.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\PycharmProjects\COMP3200-Texture-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EC5657-9303-4695-A914-6268FDD9D6D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1839D923-D6CB-4616-8E30-CA5858054B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6460020-B6F9-4319-B97D-3F281B0EF3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Algorithm</t>
   </si>
@@ -149,13 +149,7 @@
     <t>Questionable/Repeat?</t>
   </si>
   <si>
-    <t>uni (needs rerunning)</t>
-  </si>
-  <si>
     <t>CSV / Confusion Matrix Missing</t>
-  </si>
-  <si>
-    <t>desktop</t>
   </si>
   <si>
     <t>No Noise</t>
@@ -226,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,12 +253,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -281,12 +269,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -659,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -680,89 +662,85 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,7 +1058,7 @@
   <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,61 +1086,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="42"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="55"/>
       <c r="AC1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="34" t="s">
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="34" t="s">
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="37"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="50"/>
       <c r="W2" s="16"/>
       <c r="X2" s="13" t="s">
         <v>16</v>
@@ -1172,7 +1150,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="52" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11"/>
@@ -1209,10 +1187,10 @@
       <c r="M3" s="5">
         <v>0.25</v>
       </c>
-      <c r="N3" s="32">
+      <c r="N3" s="29">
         <v>0.4</v>
       </c>
-      <c r="O3" s="32">
+      <c r="O3" s="29">
         <v>0.6</v>
       </c>
       <c r="P3" s="7">
@@ -1247,74 +1225,74 @@
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="19">
         <v>0.77184151785714195</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="28">
         <v>0.82091517857142804</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="21">
         <v>0.76969866071428505</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="21">
         <v>0.80848214285714204</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="22">
         <v>0.630479910714285</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="22">
         <v>7.1395089285714197E-2</v>
       </c>
-      <c r="I4" s="24">
-        <v>0.726897321428571</v>
-      </c>
-      <c r="J4" s="25">
+      <c r="I4" s="22">
+        <v>0.72658482142857095</v>
+      </c>
+      <c r="J4" s="23">
         <v>9.3850446428571405E-2</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="23">
         <v>8.7522321428571401E-2</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="23">
         <v>8.9386160714285706E-2</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="22">
         <v>3.5758928571428497E-2</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="22">
         <v>0.120658482142857</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="22">
         <v>0.25041294642857098</v>
       </c>
-      <c r="P4" s="26">
+      <c r="P4" s="24">
         <v>3.6171874999999999E-2</v>
       </c>
-      <c r="Q4" s="26">
+      <c r="Q4" s="24">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="R4" s="26">
+      <c r="R4" s="24">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="S4" s="26">
+      <c r="S4" s="24">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="T4" s="26">
+      <c r="T4" s="24">
         <v>7.2421874999999997E-2</v>
       </c>
-      <c r="U4" s="26">
+      <c r="U4" s="24">
         <v>3.92299107142857E-2</v>
       </c>
-      <c r="V4" s="26">
+      <c r="V4" s="24">
         <v>0.678448660714285</v>
       </c>
-      <c r="W4" s="26">
+      <c r="W4" s="24">
         <v>0.43547991071428499</v>
       </c>
-      <c r="X4" s="26">
+      <c r="X4" s="24">
         <v>0.74790178571428501</v>
       </c>
       <c r="AC4" s="2" t="s">
@@ -1322,147 +1300,147 @@
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="25">
         <v>0.52756696428571404</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="23">
         <v>0.58102678571428501</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="23">
         <v>0.59507812500000001</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="23">
         <v>0.65741071428571396</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="23">
         <v>0.275223214285714</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="23">
         <v>8.1551339285714203E-2</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="23">
         <v>0.147555803571428</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="23">
         <v>0.123950892857142</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="23">
         <v>9.4944196428571395E-2</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="23">
         <v>7.9765625000000007E-2</v>
       </c>
-      <c r="M5" s="25">
+      <c r="M5" s="23">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="N5" s="25">
+      <c r="N5" s="23">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="O5" s="25">
+      <c r="O5" s="23">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="P5" s="25">
+      <c r="P5" s="23">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="Q5" s="25">
+      <c r="Q5" s="23">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="R5" s="25">
+      <c r="R5" s="23">
         <v>6.2053571428571402E-2</v>
       </c>
-      <c r="S5" s="25">
+      <c r="S5" s="23">
         <v>5.5145089285714197E-2</v>
       </c>
-      <c r="T5" s="25">
+      <c r="T5" s="23">
         <v>0.143649553571428</v>
       </c>
-      <c r="U5" s="25">
+      <c r="U5" s="23">
         <v>0.10940848214285701</v>
       </c>
-      <c r="V5" s="25">
+      <c r="V5" s="23">
         <v>0.18966517857142801</v>
       </c>
-      <c r="W5" s="25">
+      <c r="W5" s="23">
         <v>7.5792410714285705E-2</v>
       </c>
-      <c r="X5" s="25">
+      <c r="X5" s="23">
         <v>0.52964378720238003</v>
       </c>
       <c r="AC5" s="2"/>
     </row>
     <row r="6" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="25">
         <v>0.77354910714285696</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <v>0.82244419642857103</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="23">
         <v>0.84409598214285697</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="23">
         <v>0.82195312499999995</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="23">
         <v>0.75100446428571399</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="23">
         <v>9.3035714285714194E-2</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="23">
         <v>0.162276785714285</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="23">
         <v>0.45821428571428502</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="23">
         <v>7.6540178571428502E-2</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="23">
         <v>0.104040178571428</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="23">
         <v>4.0468749999999998E-2</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="23">
         <v>0.16383928571428499</v>
       </c>
-      <c r="O6" s="25">
+      <c r="O6" s="23">
         <v>0.33974330357142801</v>
       </c>
-      <c r="P6" s="25">
+      <c r="P6" s="23">
         <v>0.23513392857142801</v>
       </c>
-      <c r="Q6" s="25">
+      <c r="Q6" s="23">
         <v>3.5591517857142797E-2</v>
       </c>
-      <c r="R6" s="25">
+      <c r="R6" s="23">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="S6" s="25">
+      <c r="S6" s="23">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="T6" s="25">
+      <c r="T6" s="23">
         <v>6.6718749999999993E-2</v>
       </c>
-      <c r="U6" s="25">
+      <c r="U6" s="23">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="V6" s="25">
+      <c r="V6" s="23">
         <v>0.52712053571428497</v>
       </c>
-      <c r="W6" s="25">
+      <c r="W6" s="23">
         <v>0.289419642857142</v>
       </c>
-      <c r="X6" s="25">
+      <c r="X6" s="23">
         <v>0.81271391369047596</v>
       </c>
       <c r="AC6" s="3" t="s">
@@ -1470,74 +1448,74 @@
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="23">
         <v>0.91660714285714195</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="23">
         <v>0.94188616071428499</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="23">
         <v>0.92286830357142802</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="23">
         <v>0.92715401785714202</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="23">
         <v>0.93203124999999998</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="23">
         <v>0.90441964285714205</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="23">
         <v>0.92535714285714199</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="23">
         <v>0.92809151785714195</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="23">
         <v>0.912488839285714</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="23">
         <v>0.91015625</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="23">
         <v>5.68080357142857E-2</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="23">
         <v>0.4</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7" s="23">
         <v>0.63656250000000003</v>
       </c>
-      <c r="P7" s="25">
+      <c r="P7" s="23">
         <v>0.14849330357142801</v>
       </c>
-      <c r="Q7" s="25">
+      <c r="Q7" s="23">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="R7" s="25">
+      <c r="R7" s="23">
         <v>0.91092633928571398</v>
       </c>
-      <c r="S7" s="25">
+      <c r="S7" s="23">
         <v>0.785680803571428</v>
       </c>
-      <c r="T7" s="25">
+      <c r="T7" s="23">
         <v>0.93053571428571402</v>
       </c>
-      <c r="U7" s="25">
+      <c r="U7" s="23">
         <v>0.92069196428571398</v>
       </c>
-      <c r="V7" s="25">
+      <c r="V7" s="23">
         <v>0.93553571428571403</v>
       </c>
-      <c r="W7" s="25">
+      <c r="W7" s="23">
         <v>0.93831473214285699</v>
       </c>
-      <c r="X7" s="25">
+      <c r="X7" s="23">
         <v>0.85184709821428495</v>
       </c>
       <c r="AC7" s="18" t="s">
@@ -1545,266 +1523,283 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="26">
         <v>0.74972098214285698</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="27">
         <v>0.78465401785714195</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="27">
         <v>0.822600446428571</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="29">
+      <c r="F8" s="27">
+        <v>0.84308035714285701</v>
+      </c>
+      <c r="G8" s="27">
         <v>0.66551339285714195</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="27">
         <v>0.93906250000000002</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="27">
+        <v>0.66171875000000002</v>
+      </c>
+      <c r="J8" s="27">
+        <v>0.68694196428571397</v>
+      </c>
+      <c r="K8" s="27">
+        <v>0.72868303571428505</v>
+      </c>
+      <c r="L8" s="27">
+        <v>0.72834821428571395</v>
+      </c>
+      <c r="M8" s="27">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="N8" s="27">
+        <v>6.6183035714285701E-2</v>
+      </c>
+      <c r="O8" s="27">
+        <v>0.44034598214285697</v>
+      </c>
+      <c r="P8" s="27">
+        <v>0.28069196428571402</v>
+      </c>
+      <c r="Q8" s="27">
+        <v>0.11289062499999999</v>
+      </c>
+      <c r="R8" s="27">
+        <v>0.92991071428571404</v>
+      </c>
+      <c r="S8" s="27">
+        <v>0.21601562499999999</v>
+      </c>
+      <c r="T8" s="27">
+        <v>0.87834821428571397</v>
+      </c>
+      <c r="U8" s="27">
+        <v>0.93839285714285703</v>
+      </c>
+      <c r="V8" s="27">
+        <v>0.84196428571428505</v>
+      </c>
+      <c r="W8" s="27">
+        <v>0.84787946428571404</v>
+      </c>
+      <c r="X8" s="27">
+        <v>0.79827867445054901</v>
+      </c>
+      <c r="AC8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="30">
-        <v>0.1140625</v>
-      </c>
-      <c r="K8" s="29">
-        <v>0.72868303571428505</v>
-      </c>
-      <c r="L8" s="29">
-        <v>0.72834821428571395</v>
-      </c>
-      <c r="M8" s="29">
-        <v>3.5714285714285698E-2</v>
-      </c>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="29">
-        <v>0.28069196428571402</v>
-      </c>
-      <c r="Q8" s="29">
-        <v>0.11289062499999999</v>
-      </c>
-      <c r="R8" s="29">
-        <v>0.92991071428571404</v>
-      </c>
-      <c r="S8" s="29">
-        <v>0.21601562499999999</v>
-      </c>
-      <c r="T8" s="29">
-        <v>0.85323660714285698</v>
-      </c>
-      <c r="U8" s="29">
-        <v>0.12756696428571401</v>
-      </c>
-      <c r="V8" s="29">
-        <v>0.84196428571428505</v>
-      </c>
-      <c r="W8" s="29">
-        <v>0.84787946428571404</v>
-      </c>
-      <c r="X8" s="29">
-        <v>0.79827867445054901</v>
-      </c>
-      <c r="AC8" s="22" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
+      <c r="A9" s="52"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="R10" s="12"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51" t="s">
+      <c r="H14" s="46"/>
+      <c r="I14" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="50"/>
-      <c r="I14" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="52">
+        <v>30</v>
+      </c>
+      <c r="C15" s="37">
         <v>98.43</v>
       </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47">
+      <c r="D15" s="38"/>
+      <c r="E15" s="38">
         <v>93.11</v>
       </c>
-      <c r="F15" s="47"/>
-      <c r="G15" s="58">
+      <c r="F15" s="38"/>
+      <c r="G15" s="43">
         <v>99.18</v>
       </c>
-      <c r="H15" s="58"/>
-      <c r="I15" s="56">
+      <c r="H15" s="43"/>
+      <c r="I15" s="34">
         <v>96.909970238095198</v>
       </c>
-      <c r="J15" s="57"/>
+      <c r="J15" s="35"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="I16" s="55"/>
+      <c r="I16" s="33"/>
     </row>
     <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="42"/>
+      <c r="E18" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="59"/>
-      <c r="E18" s="53" t="s">
+      <c r="H18" s="40"/>
+      <c r="I18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="F18" s="45"/>
-      <c r="G18" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="45"/>
-      <c r="I18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="52">
+        <v>30</v>
+      </c>
+      <c r="C19" s="37">
         <v>98.84</v>
       </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47">
+      <c r="D19" s="38"/>
+      <c r="E19" s="38">
         <v>86.41</v>
       </c>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47">
+      <c r="F19" s="38"/>
+      <c r="G19" s="38">
         <v>97.69</v>
       </c>
-      <c r="H19" s="47"/>
-      <c r="I19" s="54">
+      <c r="H19" s="38"/>
+      <c r="I19" s="32">
         <v>94.83</v>
       </c>
-      <c r="J19" s="56">
+      <c r="J19" s="34">
         <v>94.440569196428498</v>
       </c>
-      <c r="K19" s="57"/>
+      <c r="K19" s="35"/>
     </row>
     <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J20" s="55"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51" t="s">
+      <c r="H21" s="46"/>
+      <c r="I21" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="50"/>
-      <c r="I21" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="52">
+        <v>31</v>
+      </c>
+      <c r="C22" s="37">
         <v>100</v>
       </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47">
+      <c r="D22" s="38"/>
+      <c r="E22" s="38">
         <v>8.9499999999999993</v>
       </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="58">
+      <c r="F22" s="38"/>
+      <c r="G22" s="43">
         <v>94.03</v>
       </c>
-      <c r="H22" s="58"/>
-      <c r="I22" s="56">
+      <c r="H22" s="43"/>
+      <c r="I22" s="34">
         <v>67.66</v>
       </c>
-      <c r="J22" s="57"/>
+      <c r="J22" s="35"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I23" s="55"/>
+      <c r="I23" s="33"/>
     </row>
     <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="41"/>
+      <c r="G25" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51" t="s">
+      <c r="H25" s="46"/>
+      <c r="I25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="36" t="s">
         <v>29</v>
-      </c>
-      <c r="F25" s="53"/>
-      <c r="G25" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" s="50"/>
-      <c r="I25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J25" s="60" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="52">
+        <v>31</v>
+      </c>
+      <c r="C26" s="37">
         <v>100</v>
       </c>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47">
+      <c r="D26" s="38"/>
+      <c r="E26" s="38">
         <v>17.86</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47">
+      <c r="F26" s="38"/>
+      <c r="G26" s="38">
         <v>87.49</v>
       </c>
-      <c r="H26" s="47"/>
-      <c r="I26" s="54">
+      <c r="H26" s="38"/>
+      <c r="I26" s="32">
         <v>62.65</v>
       </c>
-      <c r="J26" s="46">
+      <c r="J26" s="30">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="C1:X1"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:H26"/>
@@ -1821,19 +1816,6 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="C1:X1"/>
-    <mergeCell ref="C2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>